<commit_message>
Update hotel data files
</commit_message>
<xml_diff>
--- a/data/out/hotels_page_1.xlsx
+++ b/data/out/hotels_page_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,44 +463,44 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Pod 51</t>
+          <t>Maison le Bac Paris Aparthotel</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>US$2,313</t>
+          <t>US$3,735</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>7.8</t>
+          <t>8.2</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>9,904</t>
+          <t>612</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>M Social Hotel Times Square New York</t>
+          <t>Austin's Saint Lazare Hotel</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>US$4,971</t>
+          <t>US$5,908</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>8.4</t>
+          <t>8.1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -510,51 +510,51 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>9,288</t>
+          <t>2,546</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Pod Times Square</t>
+          <t>Edgar Suites Montmartre - Paul Albert</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>US$3,190</t>
+          <t>US$4,822</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>9.3</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Wonderful</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>19,833</t>
+          <t>114</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>INNSiDE by Meliá New York Nomad</t>
+          <t>Austin's Arts Et Metiers Hotel</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>US$5,447</t>
+          <t>US$6,626</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>8.4</t>
+          <t>8.2</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -564,213 +564,201 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>987</t>
+          <t>2,032</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Millennium Downtown New York</t>
+          <t>Enjoy Hostel</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>US$3,495</t>
+          <t>US$917</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>6.9</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Review score</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>4,767</t>
+          <t>5,685</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>U Hotel Fifth Avenue, Empire State Building</t>
+          <t>PARIS AUTHENTIC HOUSE, Entier 1920's villa métro Line 7</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>US$3,084</t>
+          <t>US$9,295</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>7.8</t>
+          <t>9.4</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Wonderful</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2,665</t>
+          <t>10</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Pod 39</t>
+          <t>Villa Royale Montsouris</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>US$3,273</t>
+          <t>US$4,327</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>7.6</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>9,809</t>
+          <t>283</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>The FIDI Hotel</t>
+          <t>City Inn Paris</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>US$3,405</t>
+          <t>US$835</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>8.2</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Review score</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>756</t>
+          <t>2,498</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Fairfield Inn by Marriott New York Manhattan/Financial District</t>
+          <t>Hotel 29 Lepic</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>US$3,549</t>
+          <t>US$4,759</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>8.1</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>3,184</t>
+          <t>1,995</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Residence Inn New York Downtown Manhattan/Financial District</t>
+          <t>GuestReady - Charm and Confort in the 18th</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>US$3,989</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>7.7</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>622</t>
-        </is>
-      </c>
+          <t>US$2,443</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Hotel 50 Bowery, part of JdV by Hyatt</t>
+          <t>Appart'City Collection Paris Grande Bibliothèque</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>US$4,044</t>
+          <t>US$4,294</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>8.6</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>964</t>
+          <t>1,368</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Hyatt Grand Central New York</t>
+          <t>Résidence des Poissonniers</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>US$3,801</t>
+          <t>US$3,388</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -780,19 +768,19 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2,200</t>
+          <t>33</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Royalton New York</t>
+          <t>Hôtel Soft</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>US$4,141</t>
+          <t>US$4,481</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -807,78 +795,78 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2,247</t>
+          <t>1,691</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Mondrian Park Avenue</t>
+          <t>Fauchon l'Hôtel Paris</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>US$3,668</t>
+          <t>US$19,379</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>9.3</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Review score</t>
+          <t>Wonderful</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1,320</t>
+          <t>882</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>SoHo 54</t>
+          <t>La Maison Gobert Paris Hotel Particulier</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>US$3,201</t>
+          <t>US$6,809</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>9.2</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Wonderful</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2,265</t>
+          <t>492</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Bowery Grand Hotel</t>
+          <t>Hôtel Crimée</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>US$896</t>
+          <t>US$2,998</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -888,24 +876,24 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1,246</t>
+          <t>581</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Hyatt Place NYC Chelsea</t>
+          <t>PARIS AUTHENTIC HOUSE 9 minutes by METRO RER B Gentilly to Notre-Dame de Paris</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>US$4,563</t>
+          <t>US$4,084</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>7.9</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -915,159 +903,159 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>13,098</t>
+          <t>22</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Four Points by Sheraton Manhattan Chelsea</t>
+          <t>Hollyday Studio Paris Centre Montmarte Sacré-coeur Opera Louvre</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>US$3,954</t>
+          <t>US$4,338</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>8.3</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1,229</t>
+          <t>27</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Radio Hotel</t>
+          <t>Hotel Darcet</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>US$3,890</t>
+          <t>US$3,908</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1,108</t>
+          <t>2,052</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>citizenM New York Bowery</t>
+          <t>CMG - Grands boulevards / Rex</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>US$4,336</t>
+          <t>US$6,333</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>8.7</t>
+          <t>6.8</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Review score</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2,904</t>
+          <t>39</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Candlewood Suites NYC -Times Square, an IHG Hotel</t>
+          <t>Appartement Place du Trocadéro</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>US$3,710</t>
+          <t>US$8,576</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Wonderful</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1,820</t>
+          <t>68</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Courtyard New York Downtown Manhattan/Financial District</t>
+          <t>LUXURY FLAT WITH ROOFTOP TERRACE - Paris 18</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>US$5,086</t>
+          <t>US$10,065</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>8.2</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1,320</t>
+          <t>27</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>33 Seaport Hotel New York</t>
+          <t>Best Stay Jeuneurs</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>US$7,247</t>
+          <t>US$17,598</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>8.5</t>
+          <t>8.3</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1077,24 +1065,24 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>395</t>
+          <t>538</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Aloft Manhattan Downtown - Financial District</t>
+          <t>Rent a Room - Residence Caire, Montorgueil</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>US$3,471</t>
+          <t>US$7,368</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.6</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1104,88 +1092,34 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1,202</t>
+          <t>88</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Moxy NYC Downtown</t>
+          <t>Apartments FOCH CHAMPS ELYSEES PARIS</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>US$5,453</t>
+          <t>US$40,355</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>7.8</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1,000</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Renaissance New York Harlem Hotel</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>US$4,013</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>8.1</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Very Good</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>402</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>The New Yorker, A Wyndham Hotel</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>US$3,296</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>7.7</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>13,596</t>
+          <t>4</t>
         </is>
       </c>
     </row>

</xml_diff>